<commit_message>
selenium automation email send
</commit_message>
<xml_diff>
--- a/Test_Case/TestCase.xlsx
+++ b/Test_Case/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeeva\PycharmProjects\QA_Assignment\Test_Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB43063-B350-4AE3-B839-0474AC9AC42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A086BBEC-4074-43A9-95DA-04A2557E72B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A02AE25C-5D7B-4BAB-88FA-90A82273FE53}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="118">
   <si>
     <t>SN</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>Firefox</t>
+  </si>
+  <si>
+    <t>//img[@class="global-footer-logo"]</t>
   </si>
 </sst>
 </file>
@@ -811,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0946EA59-F809-41E6-AE62-0913690DCC03}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2986,7 +2989,7 @@
         <v>40</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>14</v>

</xml_diff>